<commit_message>
Derives de taux jour 2 MAJ
</commit_message>
<xml_diff>
--- a/Derives_de_taux/xls/CalageCourbeDesTaux.xlsx
+++ b/Derives_de_taux/xls/CalageCourbeDesTaux.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
   <si>
     <t>2D</t>
   </si>
@@ -81,6 +81,12 @@
   </si>
   <si>
     <t>Diff</t>
+  </si>
+  <si>
+    <t>Plot</t>
+  </si>
+  <si>
+    <t>Value</t>
   </si>
 </sst>
 </file>
@@ -159,7 +165,6 @@
   </cellStyleXfs>
   <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -170,6 +175,7 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Milliers" xfId="1" builtinId="3"/>
@@ -468,8 +474,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:P77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -478,470 +484,476 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:16">
-      <c r="I1" s="6" t="s">
+      <c r="B1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="L1" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="M1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="N1" s="5" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="2" spans="2:16">
-      <c r="B2" t="s">
+      <c r="B2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="11">
         <v>-2.3E-3</v>
       </c>
       <c r="D2">
         <f>I2</f>
         <v>5.4794520547945206E-3</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="2">
         <f>VLOOKUP(D2,$I$2:$K$35,3,FALSE)</f>
         <v>-2.3319593430685586E-3</v>
       </c>
-      <c r="F2" s="3"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7" t="s">
+      <c r="F2" s="2"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="I2" s="7">
+      <c r="I2" s="6">
         <f>2/365</f>
         <v>5.4794520547945206E-3</v>
       </c>
-      <c r="J2" s="8">
+      <c r="J2" s="7">
         <f t="shared" ref="J2:J10" si="0">C2</f>
         <v>-2.3E-3</v>
       </c>
-      <c r="K2" s="9">
+      <c r="K2" s="8">
         <v>-2.3319593430685586E-3</v>
       </c>
-      <c r="L2" s="7">
+      <c r="L2" s="6">
         <f>EXP(-I2*K2)</f>
         <v>1.0000127779410513</v>
       </c>
-      <c r="M2" s="8">
+      <c r="M2" s="7">
         <f>(1/L2-1)/I2*360/365</f>
         <v>-2.2999999999551157E-3</v>
       </c>
-      <c r="N2" s="9">
+      <c r="N2" s="8">
         <f t="shared" ref="N2:N10" si="1">(M2-J2)*1000000</f>
         <v>4.4884235217423907E-8</v>
       </c>
     </row>
     <row r="3" spans="2:16">
-      <c r="B3" t="s">
+      <c r="B3" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="11">
         <v>-2.3E-3</v>
       </c>
       <c r="D3">
         <f>I3</f>
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="2">
         <f t="shared" ref="E3:E17" si="2">VLOOKUP(D3,$I$2:$K$35,3,FALSE)</f>
         <v>-2.3321579862787402E-3</v>
       </c>
-      <c r="F3" s="3"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7" t="s">
+      <c r="F3" s="2"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="7">
+      <c r="I3" s="6">
         <f>1/12</f>
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="J3" s="8">
+      <c r="J3" s="7">
         <f t="shared" si="0"/>
         <v>-2.3E-3</v>
       </c>
-      <c r="K3" s="9">
+      <c r="K3" s="8">
         <v>-2.3321579862787402E-3</v>
       </c>
-      <c r="L3" s="7">
+      <c r="L3" s="6">
         <f t="shared" ref="L3:L35" si="3">EXP(-(I3+$I$2)*K3)</f>
         <v>1.0002071468986831</v>
       </c>
-      <c r="M3" s="8">
+      <c r="M3" s="7">
         <f>($L$2/L3-1)/I3*360/365</f>
         <v>-2.2999999921884517E-3</v>
       </c>
-      <c r="N3" s="9">
+      <c r="N3" s="8">
         <f t="shared" si="1"/>
         <v>7.8115482832208372E-6</v>
       </c>
     </row>
     <row r="4" spans="2:16">
-      <c r="B4" t="s">
+      <c r="B4" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="11">
         <v>-1.6000000000000001E-3</v>
       </c>
       <c r="D4">
         <f>I4</f>
         <v>0.25</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="2">
         <f t="shared" si="2"/>
         <v>-1.6377664481033417E-3</v>
       </c>
-      <c r="F4" s="3"/>
-      <c r="G4" s="7">
+      <c r="F4" s="2"/>
+      <c r="G4" s="6">
         <v>3</v>
       </c>
-      <c r="H4" s="7" t="str">
+      <c r="H4" s="6" t="str">
         <f>G4&amp;"M"</f>
         <v>3M</v>
       </c>
-      <c r="I4" s="7">
+      <c r="I4" s="6">
         <f>1/4</f>
         <v>0.25</v>
       </c>
-      <c r="J4" s="8">
+      <c r="J4" s="7">
         <f t="shared" si="0"/>
         <v>-1.6000000000000001E-3</v>
       </c>
-      <c r="K4" s="9">
+      <c r="K4" s="8">
         <v>-1.6377664481033417E-3</v>
       </c>
-      <c r="L4" s="7">
+      <c r="L4" s="6">
         <f t="shared" si="3"/>
         <v>1.0004185032228037</v>
       </c>
-      <c r="M4" s="8">
+      <c r="M4" s="7">
         <f>($L$2/L4-1)/I4*360/365</f>
         <v>-1.5999999995654681E-3</v>
       </c>
-      <c r="N4" s="9">
+      <c r="N4" s="8">
         <f t="shared" si="1"/>
         <v>4.3453196769960289E-7</v>
       </c>
     </row>
     <row r="5" spans="2:16">
-      <c r="B5" t="s">
+      <c r="B5" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="11">
         <v>-1E-3</v>
       </c>
       <c r="D5">
         <f>I5</f>
         <v>0.5</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="2">
         <f t="shared" si="2"/>
         <v>-1.0284312082783202E-3</v>
       </c>
-      <c r="F5" s="3"/>
-      <c r="G5" s="7">
+      <c r="F5" s="2"/>
+      <c r="G5" s="6">
         <f>G4+3</f>
         <v>6</v>
       </c>
-      <c r="H5" s="7" t="str">
+      <c r="H5" s="6" t="str">
         <f t="shared" ref="H5" si="4">G5&amp;"M"</f>
         <v>6M</v>
       </c>
-      <c r="I5" s="7">
+      <c r="I5" s="6">
         <f>1/2</f>
         <v>0.5</v>
       </c>
-      <c r="J5" s="8">
+      <c r="J5" s="7">
         <f t="shared" si="0"/>
         <v>-1E-3</v>
       </c>
-      <c r="K5" s="9">
+      <c r="K5" s="8">
         <v>-1.0284312082783202E-3</v>
       </c>
-      <c r="L5" s="7">
+      <c r="L5" s="6">
         <f t="shared" si="3"/>
         <v>1.000519985989504</v>
       </c>
-      <c r="M5" s="8">
+      <c r="M5" s="7">
         <f>($L$2/L5-1)/I5*360/365</f>
         <v>-9.9999999999932413E-4</v>
       </c>
-      <c r="N5" s="9">
+      <c r="N5" s="8">
         <f t="shared" si="1"/>
         <v>6.7589163432746346E-10</v>
       </c>
-      <c r="P5" s="6"/>
+      <c r="P5" s="5"/>
     </row>
     <row r="6" spans="2:16">
-      <c r="B6" t="s">
+      <c r="B6" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="11">
         <v>-8.9999999999999998E-4</v>
       </c>
       <c r="D6">
         <f>I6</f>
         <v>1</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="2">
         <f t="shared" si="2"/>
         <v>-9.2064978459862625E-4</v>
       </c>
-      <c r="F6" s="5"/>
-      <c r="G6" s="7">
+      <c r="F6" s="4"/>
+      <c r="G6" s="6">
         <f>G5+6</f>
         <v>12</v>
       </c>
-      <c r="H6" s="7" t="str">
+      <c r="H6" s="6" t="str">
         <f>G6&amp;"M"</f>
         <v>12M</v>
       </c>
-      <c r="I6" s="7">
+      <c r="I6" s="6">
         <f t="shared" ref="I6:I35" si="5">G6/12</f>
         <v>1</v>
       </c>
-      <c r="J6" s="8">
+      <c r="J6" s="7">
         <f t="shared" si="0"/>
         <v>-8.9999999999999998E-4</v>
       </c>
-      <c r="K6" s="9">
+      <c r="K6" s="8">
         <v>-9.2064978459862625E-4</v>
       </c>
-      <c r="L6" s="7">
+      <c r="L6" s="6">
         <f t="shared" si="3"/>
         <v>1.0009261230282884</v>
       </c>
-      <c r="M6" s="8">
+      <c r="M6" s="7">
         <f>($L$2/L6-1)/I6*360/365</f>
         <v>-8.9999999997425017E-4</v>
       </c>
-      <c r="N6" s="9">
+      <c r="N6" s="8">
         <f t="shared" si="1"/>
         <v>2.574980159653073E-8</v>
       </c>
-      <c r="P6" s="2"/>
+      <c r="P6" s="1"/>
     </row>
     <row r="7" spans="2:16">
-      <c r="B7" t="s">
+      <c r="B7" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="11">
         <v>-1.1000000000000001E-3</v>
       </c>
       <c r="D7">
         <f>VALUE(LEFT(B7,LEN(B7)-1))</f>
         <v>2</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="2">
         <f t="shared" si="2"/>
-        <v>-3.2912434341054986E-3</v>
-      </c>
-      <c r="F7" s="3"/>
-      <c r="G7" s="7">
+        <v>-1.1038668617741555E-3</v>
+      </c>
+      <c r="F7" s="2"/>
+      <c r="G7" s="6">
         <f>G6+12</f>
         <v>24</v>
       </c>
-      <c r="H7" s="7" t="str">
+      <c r="H7" s="6" t="str">
         <f>G7&amp;"M"</f>
         <v>24M</v>
       </c>
-      <c r="I7" s="7">
+      <c r="I7" s="6">
         <f t="shared" si="5"/>
         <v>2</v>
       </c>
-      <c r="J7" s="8">
+      <c r="J7" s="7">
         <f t="shared" si="0"/>
         <v>-1.1000000000000001E-3</v>
       </c>
-      <c r="K7" s="8">
-        <v>-3.2912434341054986E-3</v>
-      </c>
-      <c r="L7" s="7">
-        <f t="shared" si="3"/>
-        <v>1.0066223525246056</v>
-      </c>
-      <c r="M7" s="11">
-        <f>($L$2-L7)/SUM($L$2:L7)</f>
-        <v>-1.0999995015548093E-3</v>
-      </c>
-      <c r="N7" s="8">
+      <c r="K7" s="7">
+        <v>-1.1038668617741555E-3</v>
+      </c>
+      <c r="L7" s="6">
+        <f t="shared" si="3"/>
+        <v>1.0022162345343788</v>
+      </c>
+      <c r="M7" s="10">
+        <f>($L$2-L7)/SUM($L$6:L7)</f>
+        <v>-1.1000000000042996E-3</v>
+      </c>
+      <c r="N7" s="7">
         <f t="shared" si="1"/>
-        <v>4.9844519072091142E-4</v>
-      </c>
-      <c r="P7" s="2"/>
+        <v>-4.2995121352085164E-9</v>
+      </c>
+      <c r="P7" s="1"/>
     </row>
     <row r="8" spans="2:16">
-      <c r="B8" t="s">
+      <c r="B8" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="11">
         <v>-1.1999999999999999E-3</v>
       </c>
       <c r="D8">
         <f t="shared" ref="D8:D17" si="6">VALUE(LEFT(B8,LEN(B8)-1))</f>
         <v>3</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="2">
         <f t="shared" si="2"/>
-        <v>-2.7942244646316098E-3</v>
-      </c>
-      <c r="F8" s="5"/>
-      <c r="G8" s="7">
+        <v>-1.2025883891720235E-3</v>
+      </c>
+      <c r="F8" s="4"/>
+      <c r="G8" s="6">
         <f t="shared" ref="G8:G35" si="7">G7+12</f>
         <v>36</v>
       </c>
-      <c r="H8" s="7" t="str">
+      <c r="H8" s="6" t="str">
         <f t="shared" ref="H8:H35" si="8">G8&amp;"M"</f>
         <v>36M</v>
       </c>
-      <c r="I8" s="7">
+      <c r="I8" s="6">
         <f t="shared" si="5"/>
         <v>3</v>
       </c>
-      <c r="J8" s="8">
+      <c r="J8" s="7">
         <f t="shared" si="0"/>
         <v>-1.1999999999999999E-3</v>
       </c>
-      <c r="K8" s="8">
-        <v>-2.7942244646316098E-3</v>
-      </c>
-      <c r="L8" s="7">
-        <f t="shared" si="3"/>
-        <v>1.008433346202795</v>
-      </c>
-      <c r="M8" s="11">
-        <f>($L$2-L8)/SUM($L$2:L8)</f>
-        <v>-1.1999999969751892E-3</v>
-      </c>
-      <c r="N8" s="8">
+      <c r="K8" s="7">
+        <v>-1.2025883891720235E-3</v>
+      </c>
+      <c r="L8" s="6">
+        <f t="shared" si="3"/>
+        <v>1.003620894349365</v>
+      </c>
+      <c r="M8" s="10">
+        <f>($L$2-L8)/SUM($L$6:L8)</f>
+        <v>-1.2000001682936866E-3</v>
+      </c>
+      <c r="N8" s="7">
         <f t="shared" si="1"/>
-        <v>3.0248106536873154E-6</v>
-      </c>
-      <c r="P8" s="2"/>
+        <v>-1.682936867121454E-4</v>
+      </c>
+      <c r="P8" s="1"/>
     </row>
     <row r="9" spans="2:16">
-      <c r="B9" t="s">
+      <c r="B9" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="11">
         <v>-2.9999999999999997E-4</v>
       </c>
       <c r="D9">
         <f t="shared" si="6"/>
         <v>4</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="2">
         <f t="shared" si="2"/>
-        <v>-6.0310516940650276E-4</v>
-      </c>
-      <c r="F9" s="3"/>
-      <c r="G9" s="7">
+        <v>-3.0319310617188617E-4</v>
+      </c>
+      <c r="F9" s="2"/>
+      <c r="G9" s="6">
         <f t="shared" si="7"/>
         <v>48</v>
       </c>
-      <c r="H9" s="7" t="str">
+      <c r="H9" s="6" t="str">
         <f t="shared" si="8"/>
         <v>48M</v>
       </c>
-      <c r="I9" s="7">
+      <c r="I9" s="6">
         <f t="shared" si="5"/>
         <v>4</v>
       </c>
-      <c r="J9" s="8">
+      <c r="J9" s="7">
         <f t="shared" si="0"/>
         <v>-2.9999999999999997E-4</v>
       </c>
-      <c r="K9" s="8">
-        <v>-6.0310516940650276E-4</v>
-      </c>
-      <c r="L9" s="7">
-        <f t="shared" si="3"/>
-        <v>1.0024186455790078</v>
-      </c>
-      <c r="M9" s="11">
-        <f>($L$2-L9)/SUM($L$2:L9)</f>
-        <v>-2.9999999670063664E-4</v>
-      </c>
-      <c r="N9" s="8">
+      <c r="K9" s="7">
+        <v>-3.0319310617188617E-4</v>
+      </c>
+      <c r="L9" s="6">
+        <f t="shared" si="3"/>
+        <v>1.0012151714800595</v>
+      </c>
+      <c r="M9" s="10">
+        <f>($L$2-L9)/SUM($L$6:L9)</f>
+        <v>-3.000000029916747E-4</v>
+      </c>
+      <c r="N9" s="7">
         <f t="shared" si="1"/>
-        <v>3.2993633324561455E-6</v>
-      </c>
-      <c r="P9" s="2"/>
+        <v>-2.9916747247907272E-6</v>
+      </c>
+      <c r="P9" s="1"/>
     </row>
     <row r="10" spans="2:16">
-      <c r="B10" t="s">
+      <c r="B10" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="11">
         <v>8.0000000000000004E-4</v>
       </c>
       <c r="D10">
         <f t="shared" si="6"/>
         <v>5</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="2">
         <f t="shared" si="2"/>
-        <v>1.4430457071467966E-3</v>
-      </c>
-      <c r="F10" s="5"/>
-      <c r="G10" s="7">
+        <v>7.9880372295564658E-4</v>
+      </c>
+      <c r="F10" s="4"/>
+      <c r="G10" s="6">
         <f t="shared" si="7"/>
         <v>60</v>
       </c>
-      <c r="H10" s="7" t="str">
+      <c r="H10" s="6" t="str">
         <f t="shared" si="8"/>
         <v>60M</v>
       </c>
-      <c r="I10" s="7">
+      <c r="I10" s="6">
         <f t="shared" si="5"/>
         <v>5</v>
       </c>
-      <c r="J10" s="8">
+      <c r="J10" s="7">
         <f t="shared" si="0"/>
         <v>8.0000000000000004E-4</v>
       </c>
-      <c r="K10" s="8">
-        <v>1.4430457071467966E-3</v>
-      </c>
-      <c r="L10" s="7">
-        <f t="shared" si="3"/>
-        <v>0.99280288851235754</v>
-      </c>
-      <c r="M10" s="11">
-        <f>($L$2-L10)/SUM($L$2:L10)</f>
-        <v>8.0000000141743533E-4</v>
-      </c>
-      <c r="N10" s="8">
+      <c r="K10" s="7">
+        <v>7.9880372295564658E-4</v>
+      </c>
+      <c r="L10" s="6">
+        <f t="shared" si="3"/>
+        <v>0.99600958731909783</v>
+      </c>
+      <c r="M10" s="10">
+        <f>($L$2-L10)/SUM($L$6:L10)</f>
+        <v>8.0000004264288221E-4</v>
+      </c>
+      <c r="N10" s="7">
         <f t="shared" si="1"/>
-        <v>1.4174352880660934E-6</v>
-      </c>
-      <c r="P10" s="2"/>
+        <v>4.2642882172420904E-5</v>
+      </c>
+      <c r="P10" s="1"/>
     </row>
     <row r="11" spans="2:16">
-      <c r="B11" t="s">
+      <c r="B11" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="11">
         <v>3.3E-3</v>
       </c>
       <c r="D11">
         <f t="shared" si="6"/>
         <v>7</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="2">
         <f t="shared" si="2"/>
-        <v>5.2547975878970135E-3</v>
-      </c>
-      <c r="F11" s="3"/>
+        <v>3.3191497736828144E-3</v>
+      </c>
+      <c r="F11" s="2"/>
       <c r="G11">
         <f t="shared" si="7"/>
         <v>72</v>
@@ -950,86 +962,86 @@
         <f t="shared" si="8"/>
         <v>72M</v>
       </c>
-      <c r="I11" s="7">
+      <c r="I11" s="6">
         <f t="shared" si="5"/>
         <v>6</v>
       </c>
-      <c r="J11" s="3"/>
-      <c r="K11" s="4">
+      <c r="J11" s="2"/>
+      <c r="K11" s="3">
         <f>FORECAST(I11,$E$10:$E$11,$D$10:$D$11)</f>
-        <v>3.3489216475219054E-3</v>
-      </c>
-      <c r="L11" s="10">
-        <f t="shared" si="3"/>
-        <v>0.98008901467566412</v>
-      </c>
-      <c r="P11" s="2"/>
+        <v>2.0589767483192309E-3</v>
+      </c>
+      <c r="L11" s="9">
+        <f t="shared" si="3"/>
+        <v>0.98771099169420684</v>
+      </c>
+      <c r="P11" s="1"/>
     </row>
     <row r="12" spans="2:16">
-      <c r="B12" t="s">
+      <c r="B12" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12" s="11">
         <v>6.7999999999999996E-3</v>
       </c>
       <c r="D12">
         <f t="shared" si="6"/>
         <v>10</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12" s="2">
         <f t="shared" si="2"/>
-        <v>9.8008287398685268E-3</v>
-      </c>
-      <c r="F12" s="5"/>
-      <c r="G12" s="7">
+        <v>6.9032105759994078E-3</v>
+      </c>
+      <c r="F12" s="4"/>
+      <c r="G12" s="6">
         <f t="shared" si="7"/>
         <v>84</v>
       </c>
-      <c r="H12" s="7" t="str">
+      <c r="H12" s="6" t="str">
         <f t="shared" si="8"/>
         <v>84M</v>
       </c>
-      <c r="I12" s="7">
+      <c r="I12" s="6">
         <f t="shared" si="5"/>
         <v>7</v>
       </c>
-      <c r="J12" s="8">
+      <c r="J12" s="7">
         <f>C11</f>
         <v>3.3E-3</v>
       </c>
-      <c r="K12" s="9">
-        <v>5.2547975878970135E-3</v>
-      </c>
-      <c r="L12" s="7">
-        <f t="shared" si="3"/>
-        <v>0.96385696057568315</v>
-      </c>
-      <c r="M12" s="11">
-        <f>($L$2-L12)/SUM($L$2:L12)</f>
-        <v>3.3000001648704732E-3</v>
-      </c>
-      <c r="N12" s="8">
+      <c r="K12" s="8">
+        <v>3.3191497736828144E-3</v>
+      </c>
+      <c r="L12" s="6">
+        <f t="shared" si="3"/>
+        <v>0.97701601453054188</v>
+      </c>
+      <c r="M12" s="10">
+        <f>($L$2-L12)/SUM($L$6:L12)</f>
+        <v>3.3000005531322167E-3</v>
+      </c>
+      <c r="N12" s="7">
         <f>(M12-J12)*1000000</f>
-        <v>1.6487047317659265E-4</v>
-      </c>
-      <c r="P12" s="2"/>
+        <v>5.5313221667893653E-4</v>
+      </c>
+      <c r="P12" s="1"/>
     </row>
     <row r="13" spans="2:16">
-      <c r="B13" t="s">
+      <c r="B13" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13" s="11">
         <v>8.6999999999999994E-3</v>
       </c>
       <c r="D13">
         <f t="shared" si="6"/>
         <v>12</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E13" s="2">
         <f t="shared" si="2"/>
-        <v>1.2056060765214821E-2</v>
-      </c>
-      <c r="F13" s="3"/>
+        <v>8.8858185046402534E-3</v>
+      </c>
+      <c r="F13" s="2"/>
       <c r="G13">
         <f t="shared" si="7"/>
         <v>96</v>
@@ -1038,37 +1050,37 @@
         <f t="shared" si="8"/>
         <v>96M</v>
       </c>
-      <c r="I13" s="7">
+      <c r="I13" s="6">
         <f t="shared" si="5"/>
         <v>8</v>
       </c>
-      <c r="J13" s="3"/>
-      <c r="K13" s="4">
+      <c r="J13" s="2"/>
+      <c r="K13" s="3">
         <f>FORECAST(I13,$E$11:$E$12,$D$11:$D$12)</f>
-        <v>6.7701413052208507E-3</v>
-      </c>
-      <c r="L13" s="10">
-        <f t="shared" si="3"/>
-        <v>0.94724431838972778</v>
-      </c>
-      <c r="P13" s="2"/>
+        <v>4.5138367077883464E-3</v>
+      </c>
+      <c r="L13" s="9">
+        <f t="shared" si="3"/>
+        <v>0.96450966397404869</v>
+      </c>
+      <c r="P13" s="1"/>
     </row>
     <row r="14" spans="2:16">
-      <c r="B14" t="s">
+      <c r="B14" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C14" s="11">
         <v>1.0699999999999999E-2</v>
       </c>
       <c r="D14">
         <f t="shared" si="6"/>
         <v>15</v>
       </c>
-      <c r="E14" s="3">
+      <c r="E14" s="2">
         <f t="shared" si="2"/>
-        <v>1.4231757578673027E-2</v>
-      </c>
-      <c r="F14" s="5"/>
+        <v>1.1005574737469513E-2</v>
+      </c>
+      <c r="F14" s="4"/>
       <c r="G14">
         <f t="shared" si="7"/>
         <v>108</v>
@@ -1077,88 +1089,88 @@
         <f t="shared" si="8"/>
         <v>108M</v>
       </c>
-      <c r="I14" s="7">
+      <c r="I14" s="6">
         <f t="shared" si="5"/>
         <v>9</v>
       </c>
-      <c r="J14" s="8"/>
-      <c r="K14" s="4">
+      <c r="J14" s="7"/>
+      <c r="K14" s="3">
         <f>FORECAST(I14,$E$11:$E$12,$D$11:$D$12)</f>
-        <v>8.2854850225446888E-3</v>
-      </c>
-      <c r="L14" s="10">
-        <f t="shared" si="3"/>
-        <v>0.92810095432855577</v>
-      </c>
-      <c r="M14" s="8"/>
-      <c r="N14" s="9"/>
-      <c r="P14" s="2"/>
+        <v>5.7085236418938775E-3</v>
+      </c>
+      <c r="L14" s="9">
+        <f t="shared" si="3"/>
+        <v>0.9498910431761437</v>
+      </c>
+      <c r="M14" s="7"/>
+      <c r="N14" s="8"/>
+      <c r="P14" s="1"/>
     </row>
     <row r="15" spans="2:16">
-      <c r="B15" t="s">
+      <c r="B15" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15" s="11">
         <v>1.2200000000000001E-2</v>
       </c>
       <c r="D15">
         <f t="shared" si="6"/>
         <v>20</v>
       </c>
-      <c r="E15" s="3">
+      <c r="E15" s="2">
         <f t="shared" si="2"/>
-        <v>1.5447189080385164E-2</v>
-      </c>
-      <c r="F15" s="3"/>
-      <c r="G15" s="7">
+        <v>1.2595383847887772E-2</v>
+      </c>
+      <c r="F15" s="2"/>
+      <c r="G15" s="6">
         <f t="shared" si="7"/>
         <v>120</v>
       </c>
-      <c r="H15" s="7" t="str">
+      <c r="H15" s="6" t="str">
         <f t="shared" si="8"/>
         <v>120M</v>
       </c>
-      <c r="I15" s="7">
+      <c r="I15" s="6">
         <f t="shared" si="5"/>
         <v>10</v>
       </c>
-      <c r="J15" s="8">
+      <c r="J15" s="7">
         <f>C12</f>
         <v>6.7999999999999996E-3</v>
       </c>
-      <c r="K15" s="9">
-        <v>9.8008287398685268E-3</v>
-      </c>
-      <c r="L15" s="7">
-        <f t="shared" si="3"/>
-        <v>0.90659270181372509</v>
-      </c>
-      <c r="M15" s="11">
-        <f>($L$2-L15)/SUM($L$2:L15)</f>
-        <v>6.8000003809427778E-3</v>
-      </c>
-      <c r="N15" s="8">
+      <c r="K15" s="8">
+        <v>6.9032105759994078E-3</v>
+      </c>
+      <c r="L15" s="6">
+        <f t="shared" si="3"/>
+        <v>0.93326141335899182</v>
+      </c>
+      <c r="M15" s="10">
+        <f>($L$2-L15)/SUM($L$6:L15)</f>
+        <v>6.800000004831986E-3</v>
+      </c>
+      <c r="N15" s="7">
         <f>(M15-J15)*1000000</f>
-        <v>3.8094277819006317E-4</v>
-      </c>
-      <c r="P15" s="2"/>
+        <v>4.8319863735213353E-6</v>
+      </c>
+      <c r="P15" s="1"/>
     </row>
     <row r="16" spans="2:16">
-      <c r="B16" t="s">
+      <c r="B16" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C16" s="11">
         <v>1.2699999999999999E-2</v>
       </c>
       <c r="D16">
         <f t="shared" si="6"/>
         <v>25</v>
       </c>
-      <c r="E16" s="3">
+      <c r="E16" s="2">
         <f t="shared" si="2"/>
-        <v>1.5495191040942184E-2</v>
-      </c>
-      <c r="F16" s="5"/>
+        <v>1.3085836391550323E-2</v>
+      </c>
+      <c r="F16" s="4"/>
       <c r="G16">
         <f t="shared" si="7"/>
         <v>132</v>
@@ -1167,72 +1179,72 @@
         <f t="shared" si="8"/>
         <v>132M</v>
       </c>
-      <c r="I16" s="7">
+      <c r="I16" s="6">
         <f t="shared" si="5"/>
         <v>11</v>
       </c>
-      <c r="J16" s="3"/>
-      <c r="K16" s="4">
+      <c r="J16" s="2"/>
+      <c r="K16" s="3">
         <f>FORECAST(I16,$E$12:$E$13,$D$12:$D$13)</f>
-        <v>1.0928444752541674E-2</v>
-      </c>
-      <c r="L16" s="10">
-        <f t="shared" si="3"/>
-        <v>0.88667854072681329</v>
-      </c>
-      <c r="P16" s="2"/>
+        <v>7.8945145403198306E-3</v>
+      </c>
+      <c r="L16" s="9">
+        <f t="shared" si="3"/>
+        <v>0.91678442870983667</v>
+      </c>
+      <c r="P16" s="1"/>
     </row>
     <row r="17" spans="2:16">
-      <c r="B17" t="s">
+      <c r="B17" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C17" s="11">
         <v>1.2800000000000001E-2</v>
       </c>
       <c r="D17">
         <f t="shared" si="6"/>
         <v>30</v>
       </c>
-      <c r="E17" s="3">
+      <c r="E17" s="2">
         <f t="shared" si="2"/>
-        <v>1.5159581323682924E-2</v>
-      </c>
-      <c r="F17" s="3"/>
-      <c r="G17" s="7">
+        <v>1.3129093662368255E-2</v>
+      </c>
+      <c r="F17" s="2"/>
+      <c r="G17" s="6">
         <f t="shared" si="7"/>
         <v>144</v>
       </c>
-      <c r="H17" s="7" t="str">
+      <c r="H17" s="6" t="str">
         <f t="shared" si="8"/>
         <v>144M</v>
       </c>
-      <c r="I17" s="7">
+      <c r="I17" s="6">
         <f t="shared" si="5"/>
         <v>12</v>
       </c>
-      <c r="J17" s="8">
+      <c r="J17" s="7">
         <f>C13</f>
         <v>8.6999999999999994E-3</v>
       </c>
-      <c r="K17" s="9">
-        <v>1.2056060765214821E-2</v>
-      </c>
-      <c r="L17" s="7">
-        <f t="shared" si="3"/>
-        <v>0.86524827527914283</v>
-      </c>
-      <c r="M17" s="11">
-        <f>($L$2-L17)/SUM($L$2:L17)</f>
-        <v>8.7000001033829197E-3</v>
-      </c>
-      <c r="N17" s="8">
+      <c r="K17" s="8">
+        <v>8.8858185046402534E-3</v>
+      </c>
+      <c r="L17" s="6">
+        <f t="shared" si="3"/>
+        <v>0.89881458512463341</v>
+      </c>
+      <c r="M17" s="10">
+        <f>($L$2-L17)/SUM($L$6:L17)</f>
+        <v>8.7000000258155089E-3</v>
+      </c>
+      <c r="N17" s="7">
         <f>(M17-J17)*1000000</f>
-        <v>1.0338292028011509E-4</v>
-      </c>
-      <c r="P17" s="2"/>
+        <v>2.581550945235378E-5</v>
+      </c>
+      <c r="P17" s="1"/>
     </row>
     <row r="18" spans="2:16">
-      <c r="F18" s="5"/>
+      <c r="F18" s="4"/>
       <c r="G18">
         <f t="shared" si="7"/>
         <v>156</v>
@@ -1241,26 +1253,26 @@
         <f t="shared" si="8"/>
         <v>156M</v>
       </c>
-      <c r="I18" s="7">
+      <c r="I18" s="6">
         <f t="shared" si="5"/>
         <v>13</v>
       </c>
-      <c r="J18" s="3"/>
-      <c r="K18" s="4">
+      <c r="J18" s="2"/>
+      <c r="K18" s="3">
         <f>FORECAST(I18,$E$13:$E$14,$D$13:$D$14)</f>
-        <v>1.2781293036367556E-2</v>
-      </c>
-      <c r="L18" s="10">
-        <f t="shared" si="3"/>
-        <v>0.84685410866350586</v>
-      </c>
-      <c r="M18" s="8"/>
-      <c r="N18" s="9"/>
-      <c r="P18" s="2"/>
+        <v>9.5924039155833394E-3</v>
+      </c>
+      <c r="L18" s="9">
+        <f t="shared" si="3"/>
+        <v>0.88271418946007263</v>
+      </c>
+      <c r="M18" s="7"/>
+      <c r="N18" s="8"/>
+      <c r="P18" s="1"/>
     </row>
     <row r="19" spans="2:16">
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
       <c r="G19">
         <f t="shared" si="7"/>
         <v>168</v>
@@ -1269,58 +1281,58 @@
         <f t="shared" si="8"/>
         <v>168M</v>
       </c>
-      <c r="I19" s="7">
+      <c r="I19" s="6">
         <f t="shared" si="5"/>
         <v>14</v>
       </c>
-      <c r="J19" s="3"/>
-      <c r="K19" s="4">
+      <c r="J19" s="2"/>
+      <c r="K19" s="3">
         <f>FORECAST(I19,$E$13:$E$14,$D$13:$D$14)</f>
-        <v>1.3506525307520291E-2</v>
-      </c>
-      <c r="L19" s="10">
-        <f t="shared" si="3"/>
-        <v>0.82764963303068928</v>
-      </c>
-      <c r="P19" s="2"/>
+        <v>1.0298989326526425E-2</v>
+      </c>
+      <c r="L19" s="9">
+        <f t="shared" si="3"/>
+        <v>0.86567798325288459</v>
+      </c>
+      <c r="P19" s="1"/>
     </row>
     <row r="20" spans="2:16">
-      <c r="F20" s="5"/>
-      <c r="G20" s="7">
+      <c r="F20" s="4"/>
+      <c r="G20" s="6">
         <f t="shared" si="7"/>
         <v>180</v>
       </c>
-      <c r="H20" s="7" t="str">
+      <c r="H20" s="6" t="str">
         <f t="shared" si="8"/>
         <v>180M</v>
       </c>
-      <c r="I20" s="7">
+      <c r="I20" s="6">
         <f t="shared" si="5"/>
         <v>15</v>
       </c>
-      <c r="J20" s="8">
+      <c r="J20" s="7">
         <f>C14</f>
         <v>1.0699999999999999E-2</v>
       </c>
-      <c r="K20" s="9">
-        <v>1.4231757578673027E-2</v>
-      </c>
-      <c r="L20" s="7">
-        <f t="shared" si="3"/>
-        <v>0.80770826331443368</v>
-      </c>
-      <c r="M20" s="11">
-        <f>($L$2-L20)/SUM($L$2:L20)</f>
-        <v>1.0700000002290138E-2</v>
-      </c>
-      <c r="N20" s="8">
+      <c r="K20" s="8">
+        <v>1.1005574737469513E-2</v>
+      </c>
+      <c r="L20" s="6">
+        <f t="shared" si="3"/>
+        <v>0.84777167927525643</v>
+      </c>
+      <c r="M20" s="10">
+        <f>($L$2-L20)/SUM($L$6:L20)</f>
+        <v>1.0700000044336737E-2</v>
+      </c>
+      <c r="N20" s="7">
         <f>(M20-J20)*1000000</f>
-        <v>2.2901385648976813E-6</v>
-      </c>
-      <c r="P20" s="2"/>
+        <v>4.4336737406447391E-5</v>
+      </c>
+      <c r="P20" s="1"/>
     </row>
     <row r="21" spans="2:16">
-      <c r="F21" s="3"/>
+      <c r="F21" s="2"/>
       <c r="G21">
         <f t="shared" si="7"/>
         <v>192</v>
@@ -1329,23 +1341,23 @@
         <f t="shared" si="8"/>
         <v>192M</v>
       </c>
-      <c r="I21" s="7">
+      <c r="I21" s="6">
         <f t="shared" si="5"/>
         <v>16</v>
       </c>
-      <c r="J21" s="3"/>
-      <c r="K21" s="4">
+      <c r="J21" s="2"/>
+      <c r="K21" s="3">
         <f>FORECAST(I21,$E$14:$E$15,$D$14:$D$15)</f>
-        <v>1.4474843879015455E-2</v>
-      </c>
-      <c r="L21" s="10">
-        <f t="shared" si="3"/>
-        <v>0.79320243200189622</v>
-      </c>
-      <c r="P21" s="2"/>
+        <v>1.1323536559553165E-2</v>
+      </c>
+      <c r="L21" s="9">
+        <f t="shared" si="3"/>
+        <v>0.83423625970041981</v>
+      </c>
+      <c r="P21" s="1"/>
     </row>
     <row r="22" spans="2:16">
-      <c r="F22" s="5"/>
+      <c r="F22" s="4"/>
       <c r="G22">
         <f t="shared" si="7"/>
         <v>204</v>
@@ -1354,23 +1366,23 @@
         <f t="shared" si="8"/>
         <v>204M</v>
       </c>
-      <c r="I22" s="7">
+      <c r="I22" s="6">
         <f t="shared" si="5"/>
         <v>17</v>
       </c>
-      <c r="J22" s="3"/>
-      <c r="K22" s="4">
+      <c r="J22" s="2"/>
+      <c r="K22" s="3">
         <f>FORECAST(I22,$E$14:$E$15,$D$14:$D$15)</f>
-        <v>1.4717930179357882E-2</v>
-      </c>
-      <c r="L22" s="10">
-        <f t="shared" si="3"/>
-        <v>0.77857849891836128</v>
-      </c>
-      <c r="P22" s="2"/>
+        <v>1.1641498381636816E-2</v>
+      </c>
+      <c r="L22" s="9">
+        <f t="shared" si="3"/>
+        <v>0.8203950704476789</v>
+      </c>
+      <c r="P22" s="1"/>
     </row>
     <row r="23" spans="2:16">
-      <c r="F23" s="3"/>
+      <c r="F23" s="2"/>
       <c r="G23">
         <f t="shared" si="7"/>
         <v>216</v>
@@ -1379,23 +1391,23 @@
         <f t="shared" si="8"/>
         <v>216M</v>
       </c>
-      <c r="I23" s="7">
+      <c r="I23" s="6">
         <f t="shared" si="5"/>
         <v>18</v>
       </c>
-      <c r="J23" s="3"/>
-      <c r="K23" s="4">
+      <c r="J23" s="2"/>
+      <c r="K23" s="3">
         <f>FORECAST(I23,$E$14:$E$15,$D$14:$D$15)</f>
-        <v>1.4961016479700308E-2</v>
-      </c>
-      <c r="L23" s="10">
-        <f t="shared" si="3"/>
-        <v>0.76385272646302882</v>
-      </c>
-      <c r="P23" s="2"/>
+        <v>1.1959460203720469E-2</v>
+      </c>
+      <c r="L23" s="9">
+        <f t="shared" si="3"/>
+        <v>0.80627063697170653</v>
+      </c>
+      <c r="P23" s="1"/>
     </row>
     <row r="24" spans="2:16">
-      <c r="F24" s="5"/>
+      <c r="F24" s="4"/>
       <c r="G24">
         <f t="shared" si="7"/>
         <v>228</v>
@@ -1404,58 +1416,58 @@
         <f t="shared" si="8"/>
         <v>228M</v>
       </c>
-      <c r="I24" s="7">
+      <c r="I24" s="6">
         <f t="shared" si="5"/>
         <v>19</v>
       </c>
-      <c r="J24" s="3"/>
-      <c r="K24" s="4">
+      <c r="J24" s="2"/>
+      <c r="K24" s="3">
         <f>FORECAST(I24,$E$14:$E$15,$D$14:$D$15)</f>
-        <v>1.5204102780042736E-2</v>
-      </c>
-      <c r="L24" s="10">
-        <f t="shared" si="3"/>
-        <v>0.74904122047064492</v>
-      </c>
-      <c r="P24" s="2"/>
+        <v>1.2277422025804119E-2</v>
+      </c>
+      <c r="L24" s="9">
+        <f t="shared" si="3"/>
+        <v>0.79188563960190994</v>
+      </c>
+      <c r="P24" s="1"/>
     </row>
     <row r="25" spans="2:16">
-      <c r="F25" s="3"/>
-      <c r="G25" s="7">
+      <c r="F25" s="2"/>
+      <c r="G25" s="6">
         <f t="shared" si="7"/>
         <v>240</v>
       </c>
-      <c r="H25" s="7" t="str">
+      <c r="H25" s="6" t="str">
         <f t="shared" si="8"/>
         <v>240M</v>
       </c>
-      <c r="I25" s="7">
+      <c r="I25" s="6">
         <f t="shared" si="5"/>
         <v>20</v>
       </c>
-      <c r="J25" s="8">
+      <c r="J25" s="7">
         <f>C15</f>
         <v>1.2200000000000001E-2</v>
       </c>
-      <c r="K25" s="9">
-        <v>1.5447189080385164E-2</v>
-      </c>
-      <c r="L25" s="7">
-        <f t="shared" si="3"/>
-        <v>0.73415990215977256</v>
-      </c>
-      <c r="M25" s="11">
-        <f>($L$2-L25)/SUM($L$2:L25)</f>
-        <v>1.2200000003148409E-2</v>
-      </c>
-      <c r="N25" s="8">
+      <c r="K25" s="8">
+        <v>1.2595383847887772E-2</v>
+      </c>
+      <c r="L25" s="6">
+        <f t="shared" si="3"/>
+        <v>0.77726285370997006</v>
+      </c>
+      <c r="M25" s="10">
+        <f>($L$2-L25)/SUM($L$6:L25)</f>
+        <v>1.2200000031435062E-2</v>
+      </c>
+      <c r="N25" s="7">
         <f>(M25-J25)*1000000</f>
-        <v>3.1484086171484904E-6</v>
-      </c>
-      <c r="P25" s="2"/>
+        <v>3.1435061151330324E-5</v>
+      </c>
+      <c r="P25" s="1"/>
     </row>
     <row r="26" spans="2:16">
-      <c r="F26" s="5"/>
+      <c r="F26" s="4"/>
       <c r="G26">
         <f>G25+12</f>
         <v>252</v>
@@ -1464,23 +1476,23 @@
         <f t="shared" si="8"/>
         <v>252M</v>
       </c>
-      <c r="I26" s="7">
+      <c r="I26" s="6">
         <f t="shared" si="5"/>
         <v>21</v>
       </c>
-      <c r="J26" s="3"/>
-      <c r="K26" s="4">
+      <c r="J26" s="2"/>
+      <c r="K26" s="3">
         <f>FORECAST(I26,$E$15:$E$16,$D$15:$D$16)</f>
-        <v>1.5456789472496568E-2</v>
-      </c>
-      <c r="L26" s="10">
-        <f t="shared" si="3"/>
-        <v>0.72276056988148274</v>
-      </c>
-      <c r="P26" s="2"/>
+        <v>1.2693474356620282E-2</v>
+      </c>
+      <c r="L26" s="9">
+        <f t="shared" si="3"/>
+        <v>0.76595449671436133</v>
+      </c>
+      <c r="P26" s="1"/>
     </row>
     <row r="27" spans="2:16">
-      <c r="F27" s="3"/>
+      <c r="F27" s="2"/>
       <c r="G27">
         <f t="shared" si="7"/>
         <v>264</v>
@@ -1489,23 +1501,23 @@
         <f t="shared" si="8"/>
         <v>264M</v>
       </c>
-      <c r="I27" s="7">
+      <c r="I27" s="6">
         <f t="shared" si="5"/>
         <v>22</v>
       </c>
-      <c r="J27" s="3"/>
-      <c r="K27" s="4">
+      <c r="J27" s="2"/>
+      <c r="K27" s="3">
         <f>FORECAST(I27,$E$15:$E$16,$D$15:$D$16)</f>
-        <v>1.5466389864607973E-2</v>
-      </c>
-      <c r="L27" s="10">
-        <f t="shared" si="3"/>
-        <v>0.71152457356326371</v>
-      </c>
-      <c r="P27" s="2"/>
+        <v>1.2791564865352793E-2</v>
+      </c>
+      <c r="L27" s="9">
+        <f t="shared" si="3"/>
+        <v>0.75466259941900404</v>
+      </c>
+      <c r="P27" s="1"/>
     </row>
     <row r="28" spans="2:16">
-      <c r="F28" s="5"/>
+      <c r="F28" s="4"/>
       <c r="G28">
         <f t="shared" si="7"/>
         <v>276</v>
@@ -1514,23 +1526,23 @@
         <f t="shared" si="8"/>
         <v>276M</v>
       </c>
-      <c r="I28" s="7">
+      <c r="I28" s="6">
         <f t="shared" si="5"/>
         <v>23</v>
       </c>
-      <c r="J28" s="3"/>
-      <c r="K28" s="4">
+      <c r="J28" s="2"/>
+      <c r="K28" s="3">
         <f>FORECAST(I28,$E$15:$E$16,$D$15:$D$16)</f>
-        <v>1.5475990256719375E-2</v>
-      </c>
-      <c r="L28" s="10">
-        <f t="shared" si="3"/>
-        <v>0.70044980211509733</v>
-      </c>
-      <c r="P28" s="2"/>
+        <v>1.2889655374085303E-2</v>
+      </c>
+      <c r="L28" s="9">
+        <f t="shared" si="3"/>
+        <v>0.74339131659335478</v>
+      </c>
+      <c r="P28" s="1"/>
     </row>
     <row r="29" spans="2:16">
-      <c r="F29" s="3"/>
+      <c r="F29" s="2"/>
       <c r="G29">
         <f t="shared" si="7"/>
         <v>288</v>
@@ -1539,58 +1551,58 @@
         <f t="shared" si="8"/>
         <v>288M</v>
       </c>
-      <c r="I29" s="7">
+      <c r="I29" s="6">
         <f t="shared" si="5"/>
         <v>24</v>
       </c>
-      <c r="J29" s="3"/>
-      <c r="K29" s="4">
+      <c r="J29" s="2"/>
+      <c r="K29" s="3">
         <f>FORECAST(I29,$E$15:$E$16,$D$15:$D$16)</f>
-        <v>1.548559064883078E-2</v>
-      </c>
-      <c r="L29" s="10">
-        <f t="shared" si="3"/>
-        <v>0.68953416807124179</v>
-      </c>
-      <c r="P29" s="2"/>
+        <v>1.2987745882817814E-2</v>
+      </c>
+      <c r="L29" s="9">
+        <f t="shared" si="3"/>
+        <v>0.7321447293167922</v>
+      </c>
+      <c r="P29" s="1"/>
     </row>
     <row r="30" spans="2:16">
-      <c r="F30" s="5"/>
-      <c r="G30" s="7">
+      <c r="F30" s="4"/>
+      <c r="G30" s="6">
         <f t="shared" si="7"/>
         <v>300</v>
       </c>
-      <c r="H30" s="7" t="str">
+      <c r="H30" s="6" t="str">
         <f t="shared" si="8"/>
         <v>300M</v>
       </c>
-      <c r="I30" s="7">
+      <c r="I30" s="6">
         <f t="shared" si="5"/>
         <v>25</v>
       </c>
-      <c r="J30" s="8">
+      <c r="J30" s="7">
         <f>C16</f>
         <v>1.2699999999999999E-2</v>
       </c>
-      <c r="K30" s="9">
-        <v>1.5495191040942184E-2</v>
-      </c>
-      <c r="L30" s="7">
-        <f t="shared" si="3"/>
-        <v>0.67877560738159659</v>
-      </c>
-      <c r="M30" s="11">
-        <f>($L$2-L30)/SUM($L$2:L30)</f>
-        <v>1.2700000681164995E-2</v>
-      </c>
-      <c r="N30" s="8">
+      <c r="K30" s="8">
+        <v>1.3085836391550323E-2</v>
+      </c>
+      <c r="L30" s="6">
+        <f t="shared" si="3"/>
+        <v>0.72092684290106557</v>
+      </c>
+      <c r="M30" s="10">
+        <f>($L$2-L30)/SUM($L$6:L30)</f>
+        <v>1.2700000015572322E-2</v>
+      </c>
+      <c r="N30" s="7">
         <f>(M30-J30)*1000000</f>
-        <v>6.811649959359567E-4</v>
-      </c>
-      <c r="P30" s="2"/>
+        <v>1.5572322945023309E-5</v>
+      </c>
+      <c r="P30" s="1"/>
     </row>
     <row r="31" spans="2:16">
-      <c r="F31" s="3"/>
+      <c r="F31" s="2"/>
       <c r="G31">
         <f t="shared" si="7"/>
         <v>312</v>
@@ -1599,23 +1611,23 @@
         <f t="shared" si="8"/>
         <v>312M</v>
       </c>
-      <c r="I31" s="7">
+      <c r="I31" s="6">
         <f t="shared" si="5"/>
         <v>26</v>
       </c>
-      <c r="J31" s="3"/>
-      <c r="K31" s="4">
+      <c r="J31" s="2"/>
+      <c r="K31" s="3">
         <f>FORECAST(I31,$E$16:$E$17,$D$16:$D$17)</f>
-        <v>1.5428069097490334E-2</v>
-      </c>
-      <c r="L31" s="10">
-        <f t="shared" si="3"/>
-        <v>0.66950654770937557</v>
-      </c>
-      <c r="P31" s="2"/>
+        <v>1.3094487845713911E-2</v>
+      </c>
+      <c r="L31" s="9">
+        <f t="shared" si="3"/>
+        <v>0.71139429805288656</v>
+      </c>
+      <c r="P31" s="1"/>
     </row>
     <row r="32" spans="2:16">
-      <c r="F32" s="5"/>
+      <c r="F32" s="4"/>
       <c r="G32">
         <f t="shared" si="7"/>
         <v>324</v>
@@ -1624,23 +1636,23 @@
         <f t="shared" si="8"/>
         <v>324M</v>
       </c>
-      <c r="I32" s="7">
+      <c r="I32" s="6">
         <f t="shared" si="5"/>
         <v>27</v>
       </c>
-      <c r="J32" s="3"/>
-      <c r="K32" s="4">
+      <c r="J32" s="2"/>
+      <c r="K32" s="3">
         <f>FORECAST(I32,$E$16:$E$17,$D$16:$D$17)</f>
-        <v>1.5360947154038481E-2</v>
-      </c>
-      <c r="L32" s="10">
-        <f t="shared" si="3"/>
-        <v>0.66045271800816774</v>
-      </c>
-      <c r="P32" s="2"/>
+        <v>1.3103139299877496E-2</v>
+      </c>
+      <c r="L32" s="9">
+        <f t="shared" si="3"/>
+        <v>0.70197565213916802</v>
+      </c>
+      <c r="P32" s="1"/>
     </row>
     <row r="33" spans="6:16">
-      <c r="F33" s="3"/>
+      <c r="F33" s="2"/>
       <c r="G33">
         <f t="shared" si="7"/>
         <v>336</v>
@@ -1649,23 +1661,23 @@
         <f t="shared" si="8"/>
         <v>336M</v>
       </c>
-      <c r="I33" s="7">
+      <c r="I33" s="6">
         <f t="shared" si="5"/>
         <v>28</v>
       </c>
-      <c r="J33" s="3"/>
-      <c r="K33" s="4">
+      <c r="J33" s="2"/>
+      <c r="K33" s="3">
         <f>FORECAST(I33,$E$16:$E$17,$D$16:$D$17)</f>
-        <v>1.529382521058663E-2</v>
-      </c>
-      <c r="L33" s="10">
-        <f t="shared" si="3"/>
-        <v>0.65160879312495057</v>
-      </c>
-      <c r="P33" s="2"/>
+        <v>1.3111790754041083E-2</v>
+      </c>
+      <c r="L33" s="9">
+        <f t="shared" si="3"/>
+        <v>0.69266972095183432</v>
+      </c>
+      <c r="P33" s="1"/>
     </row>
     <row r="34" spans="6:16">
-      <c r="F34" s="5"/>
+      <c r="F34" s="4"/>
       <c r="G34">
         <f t="shared" si="7"/>
         <v>348</v>
@@ -1674,239 +1686,239 @@
         <f t="shared" si="8"/>
         <v>348M</v>
       </c>
-      <c r="I34" s="7">
+      <c r="I34" s="6">
         <f t="shared" si="5"/>
         <v>29</v>
       </c>
-      <c r="J34" s="3"/>
-      <c r="K34" s="4">
+      <c r="J34" s="2"/>
+      <c r="K34" s="3">
         <f>FORECAST(I34,$E$16:$E$17,$D$16:$D$17)</f>
-        <v>1.5226703267134777E-2</v>
-      </c>
-      <c r="L34" s="10">
-        <f t="shared" si="3"/>
-        <v>0.6429696035410547</v>
-      </c>
-      <c r="P34" s="2"/>
+        <v>1.3120442208204668E-2</v>
+      </c>
+      <c r="L34" s="9">
+        <f t="shared" si="3"/>
+        <v>0.68347533015943385</v>
+      </c>
+      <c r="P34" s="1"/>
     </row>
     <row r="35" spans="6:16">
-      <c r="F35" s="3"/>
-      <c r="G35" s="7">
+      <c r="F35" s="2"/>
+      <c r="G35" s="6">
         <f t="shared" si="7"/>
         <v>360</v>
       </c>
-      <c r="H35" s="7" t="str">
+      <c r="H35" s="6" t="str">
         <f t="shared" si="8"/>
         <v>360M</v>
       </c>
-      <c r="I35" s="7">
+      <c r="I35" s="6">
         <f t="shared" si="5"/>
         <v>30</v>
       </c>
-      <c r="J35" s="8">
+      <c r="J35" s="7">
         <f>C17</f>
         <v>1.2800000000000001E-2</v>
       </c>
-      <c r="K35" s="9">
-        <v>1.5159581323682924E-2</v>
-      </c>
-      <c r="L35" s="7">
-        <f t="shared" si="3"/>
-        <v>0.63453013053046314</v>
-      </c>
-      <c r="M35" s="11">
-        <f>($L$2-L35)/SUM($L$2:L35)</f>
-        <v>1.2799999997451402E-2</v>
-      </c>
-      <c r="N35" s="8">
+      <c r="K35" s="8">
+        <v>1.3129093662368255E-2</v>
+      </c>
+      <c r="L35" s="6">
+        <f t="shared" si="3"/>
+        <v>0.6743913152569434</v>
+      </c>
+      <c r="M35" s="10">
+        <f>($L$2-L35)/SUM($L$6:L35)</f>
+        <v>1.2800000003517893E-2</v>
+      </c>
+      <c r="N35" s="7">
         <f>(M35-J35)*1000000</f>
-        <v>-2.5485984850304177E-6</v>
-      </c>
-      <c r="P35" s="2"/>
+        <v>3.5178925744672185E-6</v>
+      </c>
+      <c r="P35" s="1"/>
     </row>
     <row r="36" spans="6:16">
-      <c r="F36" s="5"/>
-      <c r="J36" s="3"/>
-      <c r="K36" s="4"/>
+      <c r="F36" s="4"/>
+      <c r="J36" s="2"/>
+      <c r="K36" s="3"/>
     </row>
     <row r="37" spans="6:16">
-      <c r="F37" s="3"/>
-      <c r="J37" s="3"/>
-      <c r="K37" s="4"/>
+      <c r="F37" s="2"/>
+      <c r="J37" s="2"/>
+      <c r="K37" s="3"/>
     </row>
     <row r="38" spans="6:16">
-      <c r="F38" s="5"/>
-      <c r="J38" s="3"/>
-      <c r="K38" s="4"/>
+      <c r="F38" s="4"/>
+      <c r="J38" s="2"/>
+      <c r="K38" s="3"/>
     </row>
     <row r="39" spans="6:16">
-      <c r="F39" s="3"/>
-      <c r="J39" s="3"/>
-      <c r="K39" s="4"/>
+      <c r="F39" s="2"/>
+      <c r="J39" s="2"/>
+      <c r="K39" s="3"/>
     </row>
     <row r="40" spans="6:16">
-      <c r="F40" s="5"/>
-      <c r="J40" s="3"/>
-      <c r="K40" s="4"/>
+      <c r="F40" s="4"/>
+      <c r="J40" s="2"/>
+      <c r="K40" s="3"/>
     </row>
     <row r="41" spans="6:16">
-      <c r="F41" s="3"/>
-      <c r="J41" s="3"/>
-      <c r="K41" s="4"/>
+      <c r="F41" s="2"/>
+      <c r="J41" s="2"/>
+      <c r="K41" s="3"/>
     </row>
     <row r="42" spans="6:16">
-      <c r="F42" s="5"/>
-      <c r="J42" s="3"/>
-      <c r="K42" s="4"/>
+      <c r="F42" s="4"/>
+      <c r="J42" s="2"/>
+      <c r="K42" s="3"/>
     </row>
     <row r="43" spans="6:16">
-      <c r="F43" s="3"/>
-      <c r="J43" s="3"/>
-      <c r="K43" s="4"/>
+      <c r="F43" s="2"/>
+      <c r="J43" s="2"/>
+      <c r="K43" s="3"/>
     </row>
     <row r="44" spans="6:16">
-      <c r="F44" s="5"/>
-      <c r="J44" s="3"/>
-      <c r="K44" s="4"/>
+      <c r="F44" s="4"/>
+      <c r="J44" s="2"/>
+      <c r="K44" s="3"/>
     </row>
     <row r="45" spans="6:16">
-      <c r="F45" s="3"/>
-      <c r="J45" s="3"/>
-      <c r="K45" s="4"/>
+      <c r="F45" s="2"/>
+      <c r="J45" s="2"/>
+      <c r="K45" s="3"/>
     </row>
     <row r="46" spans="6:16">
-      <c r="F46" s="5"/>
-      <c r="J46" s="3"/>
-      <c r="K46" s="4"/>
+      <c r="F46" s="4"/>
+      <c r="J46" s="2"/>
+      <c r="K46" s="3"/>
     </row>
     <row r="47" spans="6:16">
-      <c r="F47" s="3"/>
-      <c r="J47" s="3"/>
-      <c r="K47" s="4"/>
+      <c r="F47" s="2"/>
+      <c r="J47" s="2"/>
+      <c r="K47" s="3"/>
     </row>
     <row r="48" spans="6:16">
-      <c r="F48" s="5"/>
-      <c r="J48" s="3"/>
-      <c r="K48" s="4"/>
+      <c r="F48" s="4"/>
+      <c r="J48" s="2"/>
+      <c r="K48" s="3"/>
     </row>
     <row r="49" spans="6:11">
-      <c r="F49" s="3"/>
-      <c r="J49" s="3"/>
-      <c r="K49" s="4"/>
+      <c r="F49" s="2"/>
+      <c r="J49" s="2"/>
+      <c r="K49" s="3"/>
     </row>
     <row r="50" spans="6:11">
-      <c r="F50" s="5"/>
-      <c r="J50" s="3"/>
-      <c r="K50" s="4"/>
+      <c r="F50" s="4"/>
+      <c r="J50" s="2"/>
+      <c r="K50" s="3"/>
     </row>
     <row r="51" spans="6:11">
-      <c r="F51" s="3"/>
-      <c r="J51" s="3"/>
-      <c r="K51" s="4"/>
+      <c r="F51" s="2"/>
+      <c r="J51" s="2"/>
+      <c r="K51" s="3"/>
     </row>
     <row r="52" spans="6:11">
-      <c r="F52" s="5"/>
-      <c r="J52" s="3"/>
-      <c r="K52" s="4"/>
+      <c r="F52" s="4"/>
+      <c r="J52" s="2"/>
+      <c r="K52" s="3"/>
     </row>
     <row r="53" spans="6:11">
-      <c r="F53" s="3"/>
-      <c r="J53" s="3"/>
-      <c r="K53" s="4"/>
+      <c r="F53" s="2"/>
+      <c r="J53" s="2"/>
+      <c r="K53" s="3"/>
     </row>
     <row r="54" spans="6:11">
-      <c r="F54" s="5"/>
-      <c r="J54" s="3"/>
-      <c r="K54" s="4"/>
+      <c r="F54" s="4"/>
+      <c r="J54" s="2"/>
+      <c r="K54" s="3"/>
     </row>
     <row r="55" spans="6:11">
-      <c r="F55" s="3"/>
-      <c r="J55" s="3"/>
-      <c r="K55" s="4"/>
+      <c r="F55" s="2"/>
+      <c r="J55" s="2"/>
+      <c r="K55" s="3"/>
     </row>
     <row r="56" spans="6:11">
-      <c r="F56" s="5"/>
-      <c r="J56" s="3"/>
-      <c r="K56" s="4"/>
+      <c r="F56" s="4"/>
+      <c r="J56" s="2"/>
+      <c r="K56" s="3"/>
     </row>
     <row r="57" spans="6:11">
-      <c r="F57" s="3"/>
-      <c r="J57" s="3"/>
-      <c r="K57" s="4"/>
+      <c r="F57" s="2"/>
+      <c r="J57" s="2"/>
+      <c r="K57" s="3"/>
     </row>
     <row r="58" spans="6:11">
-      <c r="F58" s="5"/>
-      <c r="J58" s="3"/>
-      <c r="K58" s="4"/>
+      <c r="F58" s="4"/>
+      <c r="J58" s="2"/>
+      <c r="K58" s="3"/>
     </row>
     <row r="59" spans="6:11">
-      <c r="F59" s="3"/>
-      <c r="J59" s="3"/>
-      <c r="K59" s="4"/>
+      <c r="F59" s="2"/>
+      <c r="J59" s="2"/>
+      <c r="K59" s="3"/>
     </row>
     <row r="60" spans="6:11">
-      <c r="F60" s="5"/>
-      <c r="J60" s="3"/>
-      <c r="K60" s="4"/>
+      <c r="F60" s="4"/>
+      <c r="J60" s="2"/>
+      <c r="K60" s="3"/>
     </row>
     <row r="61" spans="6:11">
-      <c r="F61" s="3"/>
-      <c r="J61" s="3"/>
-      <c r="K61" s="4"/>
+      <c r="F61" s="2"/>
+      <c r="J61" s="2"/>
+      <c r="K61" s="3"/>
     </row>
     <row r="62" spans="6:11">
-      <c r="F62" s="5"/>
-      <c r="J62" s="3"/>
-      <c r="K62" s="4"/>
+      <c r="F62" s="4"/>
+      <c r="J62" s="2"/>
+      <c r="K62" s="3"/>
     </row>
     <row r="63" spans="6:11">
-      <c r="F63" s="3"/>
-      <c r="J63" s="3"/>
-      <c r="K63" s="4"/>
+      <c r="F63" s="2"/>
+      <c r="J63" s="2"/>
+      <c r="K63" s="3"/>
     </row>
     <row r="64" spans="6:11">
-      <c r="F64" s="5"/>
-      <c r="J64" s="3"/>
-      <c r="K64" s="4"/>
+      <c r="F64" s="4"/>
+      <c r="J64" s="2"/>
+      <c r="K64" s="3"/>
     </row>
     <row r="65" spans="6:6">
-      <c r="F65" s="3"/>
+      <c r="F65" s="2"/>
     </row>
     <row r="66" spans="6:6">
-      <c r="F66" s="5"/>
+      <c r="F66" s="4"/>
     </row>
     <row r="67" spans="6:6">
-      <c r="F67" s="3"/>
+      <c r="F67" s="2"/>
     </row>
     <row r="68" spans="6:6">
-      <c r="F68" s="5"/>
+      <c r="F68" s="4"/>
     </row>
     <row r="69" spans="6:6">
-      <c r="F69" s="3"/>
+      <c r="F69" s="2"/>
     </row>
     <row r="70" spans="6:6">
-      <c r="F70" s="5"/>
+      <c r="F70" s="4"/>
     </row>
     <row r="71" spans="6:6">
-      <c r="F71" s="3"/>
+      <c r="F71" s="2"/>
     </row>
     <row r="72" spans="6:6">
-      <c r="F72" s="5"/>
+      <c r="F72" s="4"/>
     </row>
     <row r="73" spans="6:6">
-      <c r="F73" s="3"/>
+      <c r="F73" s="2"/>
     </row>
     <row r="74" spans="6:6">
-      <c r="F74" s="5"/>
+      <c r="F74" s="4"/>
     </row>
     <row r="75" spans="6:6">
-      <c r="F75" s="3"/>
+      <c r="F75" s="2"/>
     </row>
     <row r="76" spans="6:6">
-      <c r="F76" s="5"/>
+      <c r="F76" s="4"/>
     </row>
     <row r="77" spans="6:6">
-      <c r="F77" s="3"/>
+      <c r="F77" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>